<commit_message>
- Project Report All most done
</commit_message>
<xml_diff>
--- a/tests/Projet_details/Project Report Data - Copy.xlsx
+++ b/tests/Projet_details/Project Report Data - Copy.xlsx
@@ -885,8 +885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B8" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12:E16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B79" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
1 -- Project Report Improvment needed 2. Some Changes needed
</commit_message>
<xml_diff>
--- a/tests/Projet_details/Project Report Data - Copy.xlsx
+++ b/tests/Projet_details/Project Report Data - Copy.xlsx
@@ -885,8 +885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B79" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>